<commit_message>
error solve ifrs list
</commit_message>
<xml_diff>
--- a/data/ifrs/AJ네트웍스.xlsx
+++ b/data/ifrs/AJ네트웍스.xlsx
@@ -624,103 +624,97 @@
         <v>35</v>
       </c>
       <c r="D2">
-        <v>2062060</v>
+        <v>10112</v>
       </c>
       <c r="E2">
-        <v>250251</v>
+        <v>770</v>
       </c>
       <c r="F2">
-        <v>250251</v>
+        <v>770</v>
       </c>
       <c r="G2">
-        <v>278750</v>
+        <v>364</v>
       </c>
       <c r="H2">
-        <v>233944</v>
+        <v>281</v>
       </c>
       <c r="I2">
-        <v>230825</v>
+        <v>166</v>
       </c>
       <c r="J2">
-        <v>3119</v>
+        <v>115</v>
       </c>
       <c r="K2">
-        <v>2304230</v>
+        <v>14379</v>
       </c>
       <c r="L2">
-        <v>623348</v>
+        <v>11546</v>
       </c>
       <c r="M2">
-        <v>1680882</v>
+        <v>2833</v>
       </c>
       <c r="N2">
-        <v>1621817</v>
+        <v>1616</v>
       </c>
       <c r="O2">
-        <v>59065</v>
+        <v>1216</v>
       </c>
       <c r="P2">
-        <v>8975</v>
+        <v>341</v>
       </c>
       <c r="Q2">
-        <v>369754</v>
+        <v>-802</v>
       </c>
       <c r="R2">
-        <v>-328064</v>
+        <v>-321</v>
       </c>
       <c r="S2">
-        <v>-30571</v>
+        <v>1352</v>
       </c>
       <c r="T2">
-        <v>220429</v>
+        <v>371</v>
       </c>
       <c r="U2">
-        <v>149324</v>
+        <v>-1173</v>
       </c>
       <c r="V2">
-        <v>112655</v>
+        <v>10160</v>
       </c>
       <c r="W2">
-        <v>12.14</v>
+        <v>7.61</v>
       </c>
       <c r="X2">
-        <v>11.34</v>
+        <v>2.77</v>
       </c>
       <c r="Y2">
-        <v>15.06</v>
+        <v>13.05</v>
       </c>
       <c r="Z2">
-        <v>10.53</v>
+        <v>2.87</v>
       </c>
       <c r="AA2">
-        <v>37.09</v>
+        <v>407.6</v>
       </c>
       <c r="AB2">
-        <v>19379.47</v>
+        <v>439.72</v>
       </c>
       <c r="AC2">
-        <v>2713</v>
-      </c>
-      <c r="AD2">
-        <v>9.779999999999999</v>
+        <v>546</v>
       </c>
       <c r="AE2">
-        <v>21664</v>
+        <v>4743</v>
       </c>
       <c r="AF2">
-        <v>1.23</v>
+        <v>0</v>
       </c>
       <c r="AG2">
-        <v>400</v>
-      </c>
-      <c r="AH2">
-        <v>1.51</v>
+        <v>0</v>
       </c>
       <c r="AI2">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="AJ2">
-        <v>7364966850</v>
+        <v>34082240</v>
       </c>
     </row>
     <row r="3" spans="1:36">
@@ -734,103 +728,103 @@
         <v>36</v>
       </c>
       <c r="D3">
-        <v>2006535</v>
+        <v>10556</v>
       </c>
       <c r="E3">
-        <v>264134</v>
+        <v>743</v>
       </c>
       <c r="F3">
-        <v>264134</v>
+        <v>743</v>
       </c>
       <c r="G3">
-        <v>259610</v>
+        <v>383</v>
       </c>
       <c r="H3">
-        <v>190601</v>
+        <v>290</v>
       </c>
       <c r="I3">
-        <v>186946</v>
+        <v>188</v>
       </c>
       <c r="J3">
-        <v>3655</v>
+        <v>102</v>
       </c>
       <c r="K3">
-        <v>2421795</v>
+        <v>17252</v>
       </c>
       <c r="L3">
-        <v>631197</v>
+        <v>13272</v>
       </c>
       <c r="M3">
-        <v>1790598</v>
+        <v>3980</v>
       </c>
       <c r="N3">
-        <v>1728768</v>
+        <v>2628</v>
       </c>
       <c r="O3">
-        <v>61830</v>
+        <v>1352</v>
       </c>
       <c r="P3">
-        <v>8975</v>
+        <v>468</v>
       </c>
       <c r="Q3">
-        <v>400618</v>
+        <v>-1063</v>
       </c>
       <c r="R3">
-        <v>-271678</v>
+        <v>-744</v>
       </c>
       <c r="S3">
-        <v>-65735</v>
+        <v>2312</v>
       </c>
       <c r="T3">
-        <v>258802</v>
+        <v>669</v>
       </c>
       <c r="U3">
-        <v>141815</v>
+        <v>-1733</v>
       </c>
       <c r="V3">
-        <v>128740</v>
+        <v>11612</v>
       </c>
       <c r="W3">
-        <v>13.16</v>
+        <v>7.03</v>
       </c>
       <c r="X3">
-        <v>9.5</v>
+        <v>2.75</v>
       </c>
       <c r="Y3">
-        <v>11.16</v>
+        <v>8.869999999999999</v>
       </c>
       <c r="Z3">
-        <v>8.07</v>
+        <v>1.83</v>
       </c>
       <c r="AA3">
-        <v>35.25</v>
+        <v>333.46</v>
       </c>
       <c r="AB3">
-        <v>21117.88</v>
+        <v>509.19</v>
       </c>
       <c r="AC3">
-        <v>2198</v>
+        <v>477</v>
       </c>
       <c r="AD3">
-        <v>11.47</v>
+        <v>19.75</v>
       </c>
       <c r="AE3">
-        <v>23715</v>
+        <v>5613</v>
       </c>
       <c r="AF3">
-        <v>1.06</v>
+        <v>1.68</v>
       </c>
       <c r="AG3">
-        <v>420</v>
+        <v>0</v>
       </c>
       <c r="AH3">
-        <v>1.67</v>
+        <v>0</v>
       </c>
       <c r="AI3">
-        <v>16.42</v>
+        <v>0</v>
       </c>
       <c r="AJ3">
-        <v>7364966850</v>
+        <v>46822295</v>
       </c>
     </row>
     <row r="4" spans="1:36">
@@ -844,103 +838,103 @@
         <v>37</v>
       </c>
       <c r="D4">
-        <v>2018667</v>
+        <v>12539</v>
       </c>
       <c r="E4">
-        <v>292407</v>
+        <v>619</v>
       </c>
       <c r="F4">
-        <v>292407</v>
+        <v>619</v>
       </c>
       <c r="G4">
-        <v>307137</v>
+        <v>286</v>
       </c>
       <c r="H4">
-        <v>227261</v>
+        <v>171</v>
       </c>
       <c r="I4">
-        <v>224157</v>
+        <v>135</v>
       </c>
       <c r="J4">
-        <v>3104</v>
+        <v>36</v>
       </c>
       <c r="K4">
-        <v>2621743</v>
+        <v>20813</v>
       </c>
       <c r="L4">
-        <v>692113</v>
+        <v>16538</v>
       </c>
       <c r="M4">
-        <v>1929630</v>
+        <v>4275</v>
       </c>
       <c r="N4">
-        <v>1864243</v>
+        <v>2800</v>
       </c>
       <c r="O4">
-        <v>65387</v>
+        <v>1475</v>
       </c>
       <c r="P4">
-        <v>8975</v>
+        <v>468</v>
       </c>
       <c r="Q4">
-        <v>473856</v>
+        <v>-1867</v>
       </c>
       <c r="R4">
-        <v>-296587</v>
+        <v>-851</v>
       </c>
       <c r="S4">
-        <v>-86695</v>
+        <v>3202</v>
       </c>
       <c r="T4">
-        <v>241430</v>
+        <v>431</v>
       </c>
       <c r="U4">
-        <v>232427</v>
+        <v>-2298</v>
       </c>
       <c r="V4">
-        <v>152824</v>
+        <v>14544</v>
       </c>
       <c r="W4">
-        <v>14.49</v>
+        <v>4.93</v>
       </c>
       <c r="X4">
-        <v>11.26</v>
+        <v>1.36</v>
       </c>
       <c r="Y4">
-        <v>12.48</v>
+        <v>4.98</v>
       </c>
       <c r="Z4">
-        <v>9.01</v>
+        <v>0.9</v>
       </c>
       <c r="AA4">
-        <v>35.87</v>
+        <v>386.87</v>
       </c>
       <c r="AB4">
-        <v>22004.14</v>
+        <v>538.03</v>
       </c>
       <c r="AC4">
-        <v>2735</v>
+        <v>288</v>
       </c>
       <c r="AD4">
-        <v>13.18</v>
+        <v>22.54</v>
       </c>
       <c r="AE4">
-        <v>26636</v>
+        <v>5980</v>
       </c>
       <c r="AF4">
-        <v>1.35</v>
+        <v>1.09</v>
       </c>
       <c r="AG4">
-        <v>570</v>
+        <v>60</v>
       </c>
       <c r="AH4">
-        <v>1.58</v>
+        <v>0.92</v>
       </c>
       <c r="AI4">
-        <v>17.81</v>
+        <v>20.8</v>
       </c>
       <c r="AJ4">
-        <v>7033966850</v>
+        <v>46822295</v>
       </c>
     </row>
     <row r="5" spans="1:36">
@@ -954,103 +948,103 @@
         <v>38</v>
       </c>
       <c r="D5">
-        <v>2395754</v>
+        <v>8439</v>
       </c>
       <c r="E5">
-        <v>536450</v>
+        <v>224</v>
       </c>
       <c r="F5">
-        <v>536450</v>
+        <v>224</v>
       </c>
       <c r="G5">
-        <v>561960</v>
+        <v>8</v>
       </c>
       <c r="H5">
-        <v>421867</v>
+        <v>206</v>
       </c>
       <c r="I5">
-        <v>413446</v>
+        <v>150</v>
       </c>
       <c r="J5">
-        <v>8422</v>
+        <v>56</v>
       </c>
       <c r="K5">
-        <v>3017521</v>
+        <v>23542</v>
       </c>
       <c r="L5">
-        <v>872607</v>
+        <v>19071</v>
       </c>
       <c r="M5">
-        <v>2144914</v>
+        <v>4472</v>
       </c>
       <c r="N5">
-        <v>2072134</v>
+        <v>2888</v>
       </c>
       <c r="O5">
-        <v>72780</v>
+        <v>1584</v>
       </c>
       <c r="P5">
-        <v>8975</v>
+        <v>468</v>
       </c>
       <c r="Q5">
-        <v>621620</v>
+        <v>-1485</v>
       </c>
       <c r="R5">
-        <v>-493852</v>
+        <v>-894</v>
       </c>
       <c r="S5">
-        <v>-125609</v>
+        <v>1872</v>
       </c>
       <c r="T5">
-        <v>427922</v>
+        <v>527</v>
       </c>
       <c r="U5">
-        <v>193698</v>
+        <v>-2012</v>
       </c>
       <c r="V5">
-        <v>188140</v>
+        <v>16367</v>
       </c>
       <c r="W5">
-        <v>22.39</v>
+        <v>2.66</v>
       </c>
       <c r="X5">
-        <v>17.61</v>
+        <v>2.45</v>
       </c>
       <c r="Y5">
-        <v>21.01</v>
+        <v>5.27</v>
       </c>
       <c r="Z5">
-        <v>14.96</v>
+        <v>0.93</v>
       </c>
       <c r="AA5">
-        <v>40.68</v>
+        <v>426.47</v>
       </c>
       <c r="AB5">
-        <v>24536.12</v>
+        <v>564.05</v>
       </c>
       <c r="AC5">
-        <v>5421</v>
+        <v>320</v>
       </c>
       <c r="AD5">
-        <v>9.4</v>
+        <v>21.76</v>
       </c>
       <c r="AE5">
-        <v>30427</v>
+        <v>6168</v>
       </c>
       <c r="AF5">
-        <v>1.67</v>
+        <v>1.13</v>
       </c>
       <c r="AG5">
-        <v>850</v>
+        <v>86</v>
       </c>
       <c r="AH5">
-        <v>1.67</v>
+        <v>1.23</v>
       </c>
       <c r="AI5">
-        <v>14.09</v>
+        <v>26.85</v>
       </c>
       <c r="AJ5">
-        <v>6454924700</v>
+        <v>46822295</v>
       </c>
     </row>
     <row r="6" spans="1:36">
@@ -1064,97 +1058,97 @@
         <v>39</v>
       </c>
       <c r="D6">
-        <v>2437714</v>
+        <v>10567</v>
       </c>
       <c r="E6">
-        <v>588867</v>
+        <v>-213</v>
       </c>
       <c r="F6">
-        <v>588867</v>
+        <v>-213</v>
       </c>
       <c r="G6">
-        <v>611600</v>
+        <v>-495</v>
       </c>
       <c r="H6">
-        <v>443449</v>
+        <v>373</v>
       </c>
       <c r="I6">
-        <v>438909</v>
+        <v>11</v>
       </c>
       <c r="K6">
-        <v>3393572</v>
+        <v>25751</v>
       </c>
       <c r="L6">
-        <v>916041</v>
+        <v>20833</v>
       </c>
       <c r="M6">
-        <v>2477532</v>
+        <v>4918</v>
       </c>
       <c r="N6">
-        <v>2400690</v>
+        <v>2871</v>
       </c>
       <c r="P6">
-        <v>8975</v>
+        <v>468</v>
       </c>
       <c r="Q6">
-        <v>670319</v>
+        <v>-748</v>
       </c>
       <c r="R6">
-        <v>-522405</v>
+        <v>-552</v>
       </c>
       <c r="S6">
-        <v>-150902</v>
+        <v>1275</v>
       </c>
       <c r="T6">
-        <v>295564</v>
+        <v>386</v>
       </c>
       <c r="U6">
-        <v>374755</v>
+        <v>-1134</v>
       </c>
       <c r="V6">
-        <v>146671</v>
+        <v>9928</v>
       </c>
       <c r="W6">
-        <v>24.16</v>
+        <v>-2.01</v>
       </c>
       <c r="X6">
-        <v>18.19</v>
+        <v>3.53</v>
       </c>
       <c r="Y6">
-        <v>19.63</v>
+        <v>0.39</v>
       </c>
       <c r="Z6">
-        <v>13.83</v>
+        <v>1.51</v>
       </c>
       <c r="AA6">
-        <v>36.97</v>
+        <v>423.61</v>
       </c>
       <c r="AB6">
-        <v>27531.92</v>
+        <v>561.8200000000001</v>
       </c>
       <c r="AC6">
-        <v>6024</v>
+        <v>24</v>
       </c>
       <c r="AD6">
-        <v>6.42</v>
+        <v>186.12</v>
       </c>
       <c r="AE6">
-        <v>35342</v>
+        <v>6131</v>
       </c>
       <c r="AF6">
-        <v>1.09</v>
+        <v>0.73</v>
       </c>
       <c r="AG6">
-        <v>1416</v>
+        <v>100</v>
       </c>
       <c r="AH6">
-        <v>3.66</v>
+        <v>2.22</v>
       </c>
       <c r="AI6">
-        <v>21.92</v>
+        <v>413.15</v>
       </c>
       <c r="AJ6">
-        <v>5969782550</v>
+        <v>46822295</v>
       </c>
     </row>
     <row r="7" spans="1:36">
@@ -1167,87 +1161,6 @@
       <c r="C7" t="s">
         <v>40</v>
       </c>
-      <c r="D7">
-        <v>2314725</v>
-      </c>
-      <c r="E7">
-        <v>271526</v>
-      </c>
-      <c r="G7">
-        <v>300100</v>
-      </c>
-      <c r="H7">
-        <v>219616</v>
-      </c>
-      <c r="I7">
-        <v>217026</v>
-      </c>
-      <c r="K7">
-        <v>3543848</v>
-      </c>
-      <c r="L7">
-        <v>915230</v>
-      </c>
-      <c r="M7">
-        <v>2628618</v>
-      </c>
-      <c r="N7">
-        <v>2546327</v>
-      </c>
-      <c r="P7">
-        <v>8979</v>
-      </c>
-      <c r="Q7">
-        <v>453010</v>
-      </c>
-      <c r="R7">
-        <v>-310690</v>
-      </c>
-      <c r="S7">
-        <v>-106152</v>
-      </c>
-      <c r="T7">
-        <v>282087</v>
-      </c>
-      <c r="U7">
-        <v>183465</v>
-      </c>
-      <c r="W7">
-        <v>11.73</v>
-      </c>
-      <c r="X7">
-        <v>9.49</v>
-      </c>
-      <c r="Y7">
-        <v>8.77</v>
-      </c>
-      <c r="Z7">
-        <v>6.33</v>
-      </c>
-      <c r="AA7">
-        <v>34.82</v>
-      </c>
-      <c r="AC7">
-        <v>3195</v>
-      </c>
-      <c r="AD7">
-        <v>17.37</v>
-      </c>
-      <c r="AE7">
-        <v>37486</v>
-      </c>
-      <c r="AF7">
-        <v>1.48</v>
-      </c>
-      <c r="AG7">
-        <v>1419</v>
-      </c>
-      <c r="AH7">
-        <v>2.56</v>
-      </c>
-      <c r="AI7">
-        <v>39.02</v>
-      </c>
     </row>
     <row r="8" spans="1:36">
       <c r="A8" s="1">
@@ -1259,87 +1172,6 @@
       <c r="C8" t="s">
         <v>41</v>
       </c>
-      <c r="D8">
-        <v>2527738</v>
-      </c>
-      <c r="E8">
-        <v>396877</v>
-      </c>
-      <c r="G8">
-        <v>425472</v>
-      </c>
-      <c r="H8">
-        <v>309790</v>
-      </c>
-      <c r="I8">
-        <v>306028</v>
-      </c>
-      <c r="K8">
-        <v>3826390</v>
-      </c>
-      <c r="L8">
-        <v>996832</v>
-      </c>
-      <c r="M8">
-        <v>2829558</v>
-      </c>
-      <c r="N8">
-        <v>2745657</v>
-      </c>
-      <c r="P8">
-        <v>8979</v>
-      </c>
-      <c r="Q8">
-        <v>557644</v>
-      </c>
-      <c r="R8">
-        <v>-383645</v>
-      </c>
-      <c r="S8">
-        <v>-89933</v>
-      </c>
-      <c r="T8">
-        <v>308270</v>
-      </c>
-      <c r="U8">
-        <v>259147</v>
-      </c>
-      <c r="W8">
-        <v>15.7</v>
-      </c>
-      <c r="X8">
-        <v>12.26</v>
-      </c>
-      <c r="Y8">
-        <v>11.57</v>
-      </c>
-      <c r="Z8">
-        <v>8.41</v>
-      </c>
-      <c r="AA8">
-        <v>35.23</v>
-      </c>
-      <c r="AC8">
-        <v>4505</v>
-      </c>
-      <c r="AD8">
-        <v>12.52</v>
-      </c>
-      <c r="AE8">
-        <v>40421</v>
-      </c>
-      <c r="AF8">
-        <v>1.4</v>
-      </c>
-      <c r="AG8">
-        <v>1502</v>
-      </c>
-      <c r="AH8">
-        <v>2.66</v>
-      </c>
-      <c r="AI8">
-        <v>29.3</v>
-      </c>
     </row>
     <row r="9" spans="1:36">
       <c r="A9" s="1">
@@ -1350,87 +1182,6 @@
       </c>
       <c r="C9" t="s">
         <v>42</v>
-      </c>
-      <c r="D9">
-        <v>2765706</v>
-      </c>
-      <c r="E9">
-        <v>529840</v>
-      </c>
-      <c r="G9">
-        <v>565159</v>
-      </c>
-      <c r="H9">
-        <v>413080</v>
-      </c>
-      <c r="I9">
-        <v>408159</v>
-      </c>
-      <c r="K9">
-        <v>4192070</v>
-      </c>
-      <c r="L9">
-        <v>1052638</v>
-      </c>
-      <c r="M9">
-        <v>3139432</v>
-      </c>
-      <c r="N9">
-        <v>3054491</v>
-      </c>
-      <c r="P9">
-        <v>8979</v>
-      </c>
-      <c r="Q9">
-        <v>675050</v>
-      </c>
-      <c r="R9">
-        <v>-412467</v>
-      </c>
-      <c r="S9">
-        <v>-111205</v>
-      </c>
-      <c r="T9">
-        <v>333579</v>
-      </c>
-      <c r="U9">
-        <v>355498</v>
-      </c>
-      <c r="W9">
-        <v>19.16</v>
-      </c>
-      <c r="X9">
-        <v>14.94</v>
-      </c>
-      <c r="Y9">
-        <v>14.07</v>
-      </c>
-      <c r="Z9">
-        <v>10.3</v>
-      </c>
-      <c r="AA9">
-        <v>33.53</v>
-      </c>
-      <c r="AC9">
-        <v>6009</v>
-      </c>
-      <c r="AD9">
-        <v>9.390000000000001</v>
-      </c>
-      <c r="AE9">
-        <v>44967</v>
-      </c>
-      <c r="AF9">
-        <v>1.25</v>
-      </c>
-      <c r="AG9">
-        <v>1547</v>
-      </c>
-      <c r="AH9">
-        <v>2.74</v>
-      </c>
-      <c r="AI9">
-        <v>22.63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>